<commit_message>
xml ok, Nitin error
</commit_message>
<xml_diff>
--- a/0_evaluate/input_files/Nitin_rap.xlsx
+++ b/0_evaluate/input_files/Nitin_rap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\local_user\Desktop\Study\VII_semester\TDK\BCRN\0_evaluate\input_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06EA580-C246-4670-B03C-482D009E91F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835D9BAB-7EA2-40A1-8390-346A17C734A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="3" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rap_100_nM" sheetId="1" r:id="rId1"/>
@@ -7806,7 +7806,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -8402,7 +8402,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:A12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.5"/>
   <sheetData>

</xml_diff>